<commit_message>
Done. No more to learn hear
</commit_message>
<xml_diff>
--- a/CH-154 Custom Index Column.xlsx
+++ b/CH-154 Custom Index Column.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FE43428-39B3-495C-995E-467361E8E327}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{022682B0-7642-424C-97D0-AEC4FD3DA76A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-38510" yWindow="-110" windowWidth="38620" windowHeight="21100" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -65,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="7">
   <si>
     <t>Result</t>
   </si>
@@ -83,6 +83,9 @@
   </si>
   <si>
     <t>https://www.linkedin.com/in/omid-motamedisedeh-74aba166/recent-activity/all/</t>
+  </si>
+  <si>
+    <t>My first use of adding a number to the beginning and chopping off the end.</t>
   </si>
 </sst>
 </file>
@@ -1424,7 +1427,7 @@
   <dimension ref="A1:K36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N23" sqref="N23"/>
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1669,6 +1672,11 @@
         <v>6</v>
       </c>
     </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="J14" t="s">
+        <v>6</v>
+      </c>
+    </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="D16">
         <v>0</v>

</xml_diff>